<commit_message>
More Ordinal testing ... Now I need to implement it and run a few thousand regressions with it.
</commit_message>
<xml_diff>
--- a/Analysis/BasicStatisticsOfClearly-Keto-CTA_dataAndRegressionMining (version 2).xlsb.xlsx
+++ b/Analysis/BasicStatisticsOfClearly-Keto-CTA_dataAndRegressionMining (version 2).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jille\source\repos\NinerXrayBravoTwoTwo\Keto_Cta\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B002A688-BA01-49EE-ADC7-A4A2510956AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1198E849-2864-4A63-9430-A89445EC4B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="4" xr2:uid="{D0CD085A-3F8F-465F-9DED-72CF3944BED2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="5" xr2:uid="{D0CD085A-3F8F-465F-9DED-72CF3944BED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Stats" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
-    <sheet name="Comparison of Heart Scan Tools" sheetId="3" r:id="rId6"/>
+    <sheet name="GeoMean" sheetId="7" r:id="rId6"/>
+    <sheet name="Comparison of Heart Scan Tools" sheetId="3" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="281">
   <si>
     <t>Chart</t>
   </si>
@@ -1199,6 +1200,45 @@
   </si>
   <si>
     <t>regressors</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LnGeoMeanCac </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ln(Cac1/Cac0)</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Gamma          0.000   0.000     0.000   0.000       NaN     0.000   1.00000000</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Beta           3.531   0.100     0.727   0.018    0.0914     0.313   0.55945380</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Theta          2.441   0.168     0.640   0.039    0.1316     0.388   0.52624576</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Eta            5.006   0.110     0.844   0.015   -0.0923     0.214   0.39556182</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           BetaUZeta      3.291   0.084     0.637   0.015    0.1175     0.301   0.39143815</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Alpha          1.605   0.050     0.330   0.010    0.1654     0.236   0.12417564</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Omega          1.711   0.045     0.331   0.008    0.1581     0.227   0.11576800</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Zeta           2.488   0.509     0.339   0.069    0.1346     0.801   0.00002343</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac           Qangio         3.821   0.637     0.542   0.090    0.1404     0.891   0.00000074</t>
+  </si>
+  <si>
+    <t>Ln(Cac1/Cac0) vs. LnGeoMeanCac  -- BetaUZeta</t>
+  </si>
+  <si>
+    <t>Slope: 0.1175 N=52 R^2: 0.4373 p-value: 0.391438 y-int 0.2507</t>
   </si>
 </sst>
 </file>
@@ -9224,7 +9264,7 @@
           <c:x val="0.6999779342378758"/>
           <c:y val="0.79091210831452796"/>
           <c:w val="0.2197067937080274"/>
-          <c:h val="0.17307529239038003"/>
+          <c:h val="0.17040604293665518"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10393,7 +10433,7 @@
           <c:x val="8.4930162790642222E-2"/>
           <c:y val="0.47580837836394119"/>
           <c:w val="0.2276090096757907"/>
-          <c:h val="0.1735513096882759"/>
+          <c:h val="0.17086747115387937"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10425,6 +10465,651 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Ln(Cac1/Cac0) vs. LnGeoMeanCac  -- Eta </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GeoMean!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Ln(Cac1/Cac0)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>GeoMean!$B$4:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7747793674028101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6375861597263799</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4695098776853399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5343173006204802</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1886046806471899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1891883224079303</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8828101920545</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.89564703805597</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0910424533583098</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6683669929878602</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.58370634629087</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7267317333489598</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8003087024533202</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5563867342472399</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2776993581911098</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4557134063589396</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.8790873012877203</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.4957985277338004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3159542156931296</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.3946034517012498</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.4005839671817801</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.3232729418494502</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4449053811822603</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.2344586529021502</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.4722440800471199</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.4489064815265298</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.6346813941011202</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.5518571184573302</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.9126548857360497</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.9787700925704304</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.80790102518006</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.6987347416367999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.3703554008055896</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.7701788198512096</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.2191646266663101</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.4838081630380904</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.93922109855703</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.6805581723471299</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.44117392541866</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.4758654649838503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>GeoMean!$C$4:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.916290731874155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69314718055994495</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.89381787602209595</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92367083917177695</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.64802674527947501</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.72439972406404896</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.51426796795696295</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0986122886681</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.69314718055994495</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0296194171811499</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.98082925301172597</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.88238918019847301</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.81377516834856001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5040773967762699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.90672128085800396</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.92494879461726898</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.68337738896414002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.78733439561964602</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.07956409369741</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.90409545878033604</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.69937773031058104</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.76144172799617105</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.75566753754127902</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.11803037452521</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.76063742216236097</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.79017927211128902</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.70299947700295695</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.75910514835174203</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69314718055994495</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.70849275023460501</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.71393795022901896</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.70158604920580903</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.76815209420352404</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.79126503651846802</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.74329696424541603</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.86764444224637105</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.76497291513120003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.79529499384187397</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.87632747506231701</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.76935378937058796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A03-4313-9EEE-9A731CF3CD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="389935312"/>
+        <c:axId val="389952112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="389935312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="389952112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="389952112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="389935312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -16254,6 +16939,46 @@
 </file>
 
 <file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -21757,6 +22482,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -28504,6 +29745,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA3D75-6C52-ACC5-F3A8-1E3614FFD27F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -50373,8 +51655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE984BC-2DB5-48C0-A9AC-169B7C60D5F9}">
   <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O62" sqref="O62"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56111,6 +57393,677 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0E8CA0-922C-42A7-BEE3-3864D0CE7646}">
+  <dimension ref="A1:C65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>55</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>1.7747793674028101</v>
+      </c>
+      <c r="C14">
+        <v>0.916290731874155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>3.6375861597263799</v>
+      </c>
+      <c r="C15">
+        <v>0.69314718055994495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>2.4695098776853399</v>
+      </c>
+      <c r="C16">
+        <v>0.89381787602209595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>62</v>
+      </c>
+      <c r="B17">
+        <v>3.5343173006204802</v>
+      </c>
+      <c r="C17">
+        <v>0.92367083917177695</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <v>4.1886046806471899</v>
+      </c>
+      <c r="C18">
+        <v>0.64802674527947501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <v>4.1891883224079303</v>
+      </c>
+      <c r="C19">
+        <v>0.72439972406404896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>65</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>66</v>
+      </c>
+      <c r="B21">
+        <v>3.8828101920545</v>
+      </c>
+      <c r="C21">
+        <v>0.51426796795696295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>67</v>
+      </c>
+      <c r="B22">
+        <v>1.89564703805597</v>
+      </c>
+      <c r="C22">
+        <v>1.0986122886681</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>68</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>69</v>
+      </c>
+      <c r="B24">
+        <v>3.0910424533583098</v>
+      </c>
+      <c r="C24">
+        <v>0.69314718055994495</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>70</v>
+      </c>
+      <c r="B25">
+        <v>2.6683669929878602</v>
+      </c>
+      <c r="C25">
+        <v>1.0296194171811499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>71</v>
+      </c>
+      <c r="B26">
+        <v>1.58370634629087</v>
+      </c>
+      <c r="C26">
+        <v>0.98082925301172597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>72</v>
+      </c>
+      <c r="B27">
+        <v>2.7267317333489598</v>
+      </c>
+      <c r="C27">
+        <v>0.88238918019847301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>73</v>
+      </c>
+      <c r="B28">
+        <v>3.8003087024533202</v>
+      </c>
+      <c r="C28">
+        <v>0.81377516834856001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>74</v>
+      </c>
+      <c r="B29">
+        <v>1.5563867342472399</v>
+      </c>
+      <c r="C29">
+        <v>1.5040773967762699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>75</v>
+      </c>
+      <c r="B30">
+        <v>3.2776993581911098</v>
+      </c>
+      <c r="C30">
+        <v>0.90672128085800396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>76</v>
+      </c>
+      <c r="B31">
+        <v>4.4557134063589396</v>
+      </c>
+      <c r="C31">
+        <v>0.92494879461726898</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>5.8790873012877203</v>
+      </c>
+      <c r="C32">
+        <v>0.68337738896414002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>78</v>
+      </c>
+      <c r="B33">
+        <v>4.4957985277338004</v>
+      </c>
+      <c r="C33">
+        <v>0.78733439561964602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>79</v>
+      </c>
+      <c r="B34">
+        <v>4.3159542156931296</v>
+      </c>
+      <c r="C34">
+        <v>1.07956409369741</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>80</v>
+      </c>
+      <c r="B35">
+        <v>4.3946034517012498</v>
+      </c>
+      <c r="C35">
+        <v>0.90409545878033604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>81</v>
+      </c>
+      <c r="B36">
+        <v>4.4005839671817801</v>
+      </c>
+      <c r="C36">
+        <v>0.69937773031058104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>82</v>
+      </c>
+      <c r="B37">
+        <v>5.3232729418494502</v>
+      </c>
+      <c r="C37">
+        <v>0.76144172799617105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>83</v>
+      </c>
+      <c r="B38">
+        <v>5.4449053811822603</v>
+      </c>
+      <c r="C38">
+        <v>0.75566753754127902</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>84</v>
+      </c>
+      <c r="B39">
+        <v>3.2344586529021502</v>
+      </c>
+      <c r="C39">
+        <v>1.11803037452521</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>85</v>
+      </c>
+      <c r="B40">
+        <v>5.4722440800471199</v>
+      </c>
+      <c r="C40">
+        <v>0.76063742216236097</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>86</v>
+      </c>
+      <c r="B41">
+        <v>5.4489064815265298</v>
+      </c>
+      <c r="C41">
+        <v>0.79017927211128902</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>87</v>
+      </c>
+      <c r="B42">
+        <v>4.6346813941011202</v>
+      </c>
+      <c r="C42">
+        <v>0.70299947700295695</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>88</v>
+      </c>
+      <c r="B43">
+        <v>4.5518571184573302</v>
+      </c>
+      <c r="C43">
+        <v>0.75910514835174203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>89</v>
+      </c>
+      <c r="B44">
+        <v>4.9126548857360497</v>
+      </c>
+      <c r="C44">
+        <v>0.69314718055994495</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>90</v>
+      </c>
+      <c r="B45">
+        <v>5.9787700925704304</v>
+      </c>
+      <c r="C45">
+        <v>0.70849275023460501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>91</v>
+      </c>
+      <c r="B46">
+        <v>4.80790102518006</v>
+      </c>
+      <c r="C46">
+        <v>0.71393795022901896</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>92</v>
+      </c>
+      <c r="B47">
+        <v>5.6987347416367999</v>
+      </c>
+      <c r="C47">
+        <v>0.70158604920580903</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>93</v>
+      </c>
+      <c r="B48">
+        <v>5.3703554008055896</v>
+      </c>
+      <c r="C48">
+        <v>0.76815209420352404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>94</v>
+      </c>
+      <c r="B49">
+        <v>5.7701788198512096</v>
+      </c>
+      <c r="C49">
+        <v>0.79126503651846802</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>95</v>
+      </c>
+      <c r="B50">
+        <v>5.2191646266663101</v>
+      </c>
+      <c r="C50">
+        <v>0.74329696424541603</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>96</v>
+      </c>
+      <c r="B51">
+        <v>6.4838081630380904</v>
+      </c>
+      <c r="C51">
+        <v>0.86764444224637105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>97</v>
+      </c>
+      <c r="B52">
+        <v>3.93922109855703</v>
+      </c>
+      <c r="C52">
+        <v>0.76497291513120003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>98</v>
+      </c>
+      <c r="B53">
+        <v>5.6805581723471299</v>
+      </c>
+      <c r="C53">
+        <v>0.79529499384187397</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>99</v>
+      </c>
+      <c r="B54">
+        <v>5.44117392541866</v>
+      </c>
+      <c r="C54">
+        <v>0.87632747506231701</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>5.4758654649838503</v>
+      </c>
+      <c r="C55">
+        <v>0.76935378937058796</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618AF593-FCF0-49CF-96A1-B6A4A279B311}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>